<commit_message>
Se agregan opciones de generos
</commit_message>
<xml_diff>
--- a/Cantantes.xlsx
+++ b/Cantantes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enlace 3\Desktop\pagina_web\pagina_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521DA476-E68B-4E8D-AECE-4134457643E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9D2BB5-52BB-4EFC-8B08-20B10A75FCB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,29 +25,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Cantante/Banda</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Fecha de nacimiento</t>
   </si>
   <si>
-    <t>Fecha de muerte</t>
+    <t>Genero</t>
   </si>
   <si>
-    <t>Primera cancion</t>
+    <t>Datos importantes</t>
   </si>
   <si>
-    <t>Datos random</t>
+    <t>Banda/artista</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha de muerte </t>
+  </si>
+  <si>
+    <t>Primera Cancion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -64,12 +81,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF91AFEB"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -92,16 +109,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,39 +438,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F2"/>
+  <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5" t="s">
+        <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="I7" s="5"/>
+      <c r="J7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="M7" s="6"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="6"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L13" s="10"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B7:C8"/>
+    <mergeCell ref="D7:E8"/>
+    <mergeCell ref="F7:G8"/>
+    <mergeCell ref="H7:I8"/>
+    <mergeCell ref="J7:K8"/>
+    <mergeCell ref="L7:M8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <picture r:id="rId1"/>
+  <webPublishItems count="1">
+    <webPublishItem id="8421" divId="Cantantes_8421" sourceType="sheet" destinationFile="C:\Users\Enlace 3\Desktop\pagina_web\pagina_web\Genero.htm" autoRepublish="1"/>
+  </webPublishItems>
 </worksheet>
 </file>
</xml_diff>